<commit_message>
final commit add png and results
</commit_message>
<xml_diff>
--- a/data/Experiment_record_part2.xlsx
+++ b/data/Experiment_record_part2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/howechen/Project/ntu_sd6103_team_project/ntu_sd6103_data_systems_team_project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Howe's T7/Project/ntu_sd6103_team_project/ntu_sd6103_data_systems_team_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDECD976-38D0-8E40-8078-B05D9F5E1D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664B3A4E-DD29-7648-8606-BDB0365B2745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="-19640" windowWidth="29400" windowHeight="17380" xr2:uid="{91221B1A-156A-874A-9362-4845446E1592}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17380" xr2:uid="{91221B1A-156A-874A-9362-4845446E1592}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>